<commit_message>
updated BRA and NOR
</commit_message>
<xml_diff>
--- a/NOR.xlsx
+++ b/NOR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard.000\gitboyzorro5\Rsoccer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitboyzorro5\Rsoccer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3902,7 +3902,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -3946,14 +3946,14 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4001,106 +4001,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5845,10 +5745,10 @@
   <dimension ref="A1:CK241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="BD110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="BF221" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A125" activeCellId="1" sqref="CB1:CB1048576 A125:XFD125"/>
+      <selection pane="bottomRight" activeCell="A239" sqref="A239:XFD239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44861,272 +44761,272 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="146" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="146" spans="1:89" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E146">
+      <c r="E146" s="4">
         <v>1.7273000000000001</v>
       </c>
-      <c r="F146">
+      <c r="F146" s="4">
         <v>0.69469999999999998</v>
       </c>
-      <c r="G146">
+      <c r="G146" s="4">
         <v>1.0421</v>
       </c>
-      <c r="H146">
+      <c r="H146" s="4">
         <v>1.1429</v>
       </c>
-      <c r="I146">
+      <c r="I146" s="4">
         <v>1.05</v>
       </c>
-      <c r="J146">
+      <c r="J146" s="4">
         <v>1.3998999999999999</v>
       </c>
-      <c r="K146">
+      <c r="K146" s="4">
         <v>1.250473428551</v>
       </c>
-      <c r="L146">
+      <c r="L146" s="4">
         <v>1.6799429955</v>
       </c>
-      <c r="M146">
+      <c r="M146" s="4">
         <v>5.3400000000000003E-2</v>
       </c>
-      <c r="N146">
+      <c r="N146" s="4">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="O146">
+      <c r="O146" s="4">
         <v>8.9700000000000002E-2</v>
       </c>
-      <c r="P146">
+      <c r="P146" s="4">
         <v>0.11210000000000001</v>
       </c>
-      <c r="Q146">
+      <c r="Q146" s="4">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="R146">
+      <c r="R146" s="4">
         <v>7.5300000000000006E-2</v>
       </c>
-      <c r="S146">
+      <c r="S146" s="4">
         <v>5.8900000000000001E-2</v>
       </c>
-      <c r="T146">
+      <c r="T146" s="4">
         <v>7.0099999999999996E-2</v>
       </c>
-      <c r="U146">
+      <c r="U146" s="4">
         <v>9.4200000000000006E-2</v>
       </c>
-      <c r="V146">
+      <c r="V146" s="4">
         <v>1.37E-2</v>
       </c>
-      <c r="W146">
+      <c r="W146" s="4">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="X146">
+      <c r="X146" s="4">
         <v>2.92E-2</v>
       </c>
-      <c r="Y146">
+      <c r="Y146" s="4">
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="Z146">
+      <c r="Z146" s="4">
         <v>4.2200000000000001E-2</v>
       </c>
-      <c r="AA146">
+      <c r="AA146" s="4">
         <v>5.2699999999999997E-2</v>
       </c>
-      <c r="AB146">
+      <c r="AB146" s="4">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="AC146">
+      <c r="AC146" s="4">
         <v>1.8E-3</v>
       </c>
-      <c r="AD146">
+      <c r="AD146" s="4">
         <v>5.4000000000000003E-3</v>
       </c>
-      <c r="AE146">
+      <c r="AE146" s="4">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="AF146">
+      <c r="AF146" s="4">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="AG146">
+      <c r="AG146" s="4">
         <v>4.3E-3</v>
       </c>
-      <c r="AH146">
+      <c r="AH146" s="4">
         <v>1.77E-2</v>
       </c>
-      <c r="AI146">
+      <c r="AI146" s="4">
         <v>2.2200000000000001E-2</v>
       </c>
-      <c r="AJ146">
+      <c r="AJ146" s="4">
         <v>1.38E-2</v>
       </c>
-      <c r="AK146">
+      <c r="AK146" s="4">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="AL146">
+      <c r="AL146" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="AM146">
+      <c r="AM146" s="4">
         <v>1.4E-3</v>
       </c>
-      <c r="AN146">
+      <c r="AN146" s="4">
         <v>2.3E-3</v>
       </c>
-      <c r="AO146">
+      <c r="AO146" s="4">
         <v>1.9E-3</v>
       </c>
-      <c r="AP146">
+      <c r="AP146" s="4">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="AQ146">
+      <c r="AQ146" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="AR146">
+      <c r="AR146" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="AS146">
+      <c r="AS146" s="4">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="AT146">
+      <c r="AT146" s="4">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="AU146">
+      <c r="AU146" s="4">
         <v>1.9E-3</v>
       </c>
-      <c r="AV146">
+      <c r="AV146" s="4">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="AW146">
-        <v>0</v>
-      </c>
-      <c r="AX146">
+      <c r="AW146" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX146" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="AY146">
+      <c r="AY146" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="AZ146">
+      <c r="AZ146" s="4">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="BA146">
+      <c r="BA146" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="BB146">
-        <v>1E-4</v>
-      </c>
-      <c r="BC146">
-        <v>0</v>
-      </c>
-      <c r="BD146">
+      <c r="BB146" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="BC146" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD146" s="4">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="BE146">
+      <c r="BE146" s="4">
         <v>2.0999999999999999E-3</v>
       </c>
-      <c r="BF146">
+      <c r="BF146" s="4">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="BG146">
+      <c r="BG146" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="BH146">
+      <c r="BH146" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="BI146">
-        <v>0</v>
-      </c>
-      <c r="BJ146" s="3">
+      <c r="BI146" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ146" s="5">
         <v>0.28499999999999998</v>
       </c>
-      <c r="BK146" s="3">
+      <c r="BK146" s="5">
         <v>0.24</v>
       </c>
-      <c r="BL146" s="3">
+      <c r="BL146" s="5">
         <v>0.47299999999999998</v>
       </c>
-      <c r="BM146" s="3">
+      <c r="BM146" s="5">
         <v>0.55900000000000005</v>
       </c>
-      <c r="BN146" s="3">
+      <c r="BN146" s="5">
         <v>0.439</v>
       </c>
-      <c r="BO146">
+      <c r="BO146" s="4">
         <v>1.79</v>
       </c>
-      <c r="BP146">
+      <c r="BP146" s="4">
         <v>2.2799999999999998</v>
       </c>
-      <c r="BQ146" t="s">
+      <c r="BQ146" s="4" t="s">
         <v>952</v>
       </c>
-      <c r="BR146" t="s">
+      <c r="BR146" s="4" t="s">
         <v>903</v>
       </c>
-      <c r="BS146">
+      <c r="BS146" s="4">
         <v>1.91</v>
       </c>
-      <c r="BT146">
+      <c r="BT146" s="4">
         <v>1.4</v>
       </c>
-      <c r="BU146" t="s">
+      <c r="BU146" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="BV146" t="s">
+      <c r="BV146" s="4" t="s">
         <v>877</v>
       </c>
-      <c r="BW146">
+      <c r="BW146" s="4">
         <v>3.51</v>
       </c>
-      <c r="BX146">
+      <c r="BX146" s="4">
         <v>2.11</v>
       </c>
-      <c r="BY146" t="s">
+      <c r="BY146" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="BZ146" t="s">
+      <c r="BZ146" s="4" t="s">
         <v>1246</v>
       </c>
-      <c r="CA146">
+      <c r="CA146" s="4">
         <v>1.34</v>
       </c>
-      <c r="CB146">
+      <c r="CB146" s="4">
         <v>1.1399999999999999</v>
       </c>
-      <c r="CC146" t="s">
+      <c r="CC146" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="CD146" t="s">
+      <c r="CD146" s="4" t="s">
         <v>877</v>
       </c>
-      <c r="CE146">
+      <c r="CE146" s="4">
         <v>3.51</v>
       </c>
-      <c r="CF146">
+      <c r="CF146" s="4">
         <v>2.11</v>
       </c>
-      <c r="CG146" t="s">
+      <c r="CG146" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="CH146" t="s">
+      <c r="CH146" s="4" t="s">
         <v>1246</v>
       </c>
-      <c r="CI146">
+      <c r="CI146" s="4">
         <v>1.34</v>
       </c>
-      <c r="CJ146">
+      <c r="CJ146" s="4">
         <v>1.1399999999999999</v>
       </c>
-      <c r="CK146" t="s">
+      <c r="CK146" s="4" t="s">
         <v>1268</v>
       </c>
     </row>
@@ -69878,272 +69778,272 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="239" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
+    <row r="239" spans="1:89" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B239" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C239" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E239">
+      <c r="E239" s="4">
         <v>1.7273000000000001</v>
       </c>
-      <c r="F239">
+      <c r="F239" s="4">
         <v>1.3895</v>
       </c>
-      <c r="G239">
+      <c r="G239" s="4">
         <v>1.7367999999999999</v>
       </c>
-      <c r="H239">
+      <c r="H239" s="4">
         <v>1.1429</v>
       </c>
-      <c r="I239">
+      <c r="I239" s="4">
         <v>0.52500000000000002</v>
       </c>
-      <c r="J239">
+      <c r="J239" s="4">
         <v>1.2250000000000001</v>
       </c>
-      <c r="K239">
+      <c r="K239" s="4">
         <v>4.1684647622800002</v>
       </c>
-      <c r="L239">
+      <c r="L239" s="4">
         <v>0.73502756250000012</v>
       </c>
-      <c r="M239">
+      <c r="M239" s="4">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="N239">
+      <c r="N239" s="4">
         <v>3.09E-2</v>
       </c>
-      <c r="O239">
+      <c r="O239" s="4">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="P239">
+      <c r="P239" s="4">
         <v>2.2700000000000001E-2</v>
       </c>
-      <c r="Q239">
+      <c r="Q239" s="4">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="R239">
+      <c r="R239" s="4">
         <v>2E-3</v>
       </c>
-      <c r="S239">
+      <c r="S239" s="4">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="T239">
+      <c r="T239" s="4">
         <v>4.7399999999999998E-2</v>
       </c>
-      <c r="U239">
+      <c r="U239" s="4">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="V239">
+      <c r="V239" s="4">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="W239">
+      <c r="W239" s="4">
         <v>8.9599999999999999E-2</v>
       </c>
-      <c r="X239">
+      <c r="X239" s="4">
         <v>6.5799999999999997E-2</v>
       </c>
-      <c r="Y239">
+      <c r="Y239" s="4">
         <v>2.4199999999999999E-2</v>
       </c>
-      <c r="Z239">
+      <c r="Z239" s="4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="AA239">
+      <c r="AA239" s="4">
         <v>2E-3</v>
       </c>
-      <c r="AB239">
+      <c r="AB239" s="4">
         <v>4.3E-3</v>
       </c>
-      <c r="AC239">
+      <c r="AC239" s="4">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="AD239">
+      <c r="AD239" s="4">
         <v>9.3399999999999997E-2</v>
       </c>
-      <c r="AE239">
+      <c r="AE239" s="4">
         <v>6.8599999999999994E-2</v>
       </c>
-      <c r="AF239">
+      <c r="AF239" s="4">
         <v>2.52E-2</v>
       </c>
-      <c r="AG239">
+      <c r="AG239" s="4">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="AH239">
-        <v>1E-4</v>
-      </c>
-      <c r="AI239">
+      <c r="AH239" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="AI239" s="4">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="AJ239">
+      <c r="AJ239" s="4">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="AK239">
+      <c r="AK239" s="4">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="AL239">
-        <v>1E-4</v>
-      </c>
-      <c r="AM239">
+      <c r="AL239" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="AM239" s="4">
         <v>7.7799999999999994E-2</v>
       </c>
-      <c r="AN239">
+      <c r="AN239" s="4">
         <v>5.7200000000000001E-2</v>
       </c>
-      <c r="AO239">
+      <c r="AO239" s="4">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AP239">
+      <c r="AP239" s="4">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="AQ239">
+      <c r="AQ239" s="4">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="AR239">
-        <v>0</v>
-      </c>
-      <c r="AS239">
-        <v>1E-4</v>
-      </c>
-      <c r="AT239">
-        <v>1E-4</v>
-      </c>
-      <c r="AU239">
+      <c r="AR239" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS239" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="AT239" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="AU239" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="AV239">
+      <c r="AV239" s="4">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="AW239">
-        <v>0</v>
-      </c>
-      <c r="AX239">
+      <c r="AW239" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX239" s="4">
         <v>5.4100000000000002E-2</v>
       </c>
-      <c r="AY239">
+      <c r="AY239" s="4">
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="AZ239">
+      <c r="AZ239" s="4">
         <v>1.46E-2</v>
       </c>
-      <c r="BA239">
+      <c r="BA239" s="4">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="BB239">
+      <c r="BB239" s="4">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="BC239">
-        <v>1E-4</v>
-      </c>
-      <c r="BD239">
-        <v>0</v>
-      </c>
-      <c r="BE239">
-        <v>0</v>
-      </c>
-      <c r="BF239">
-        <v>0</v>
-      </c>
-      <c r="BG239">
-        <v>0</v>
-      </c>
-      <c r="BH239">
-        <v>0</v>
-      </c>
-      <c r="BI239">
-        <v>0</v>
-      </c>
-      <c r="BJ239" s="3">
+      <c r="BC239" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="BD239" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE239" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF239" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG239" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH239" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI239" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ239" s="5">
         <v>0.79100000000000004</v>
       </c>
-      <c r="BK239" s="3">
+      <c r="BK239" s="5">
         <v>5.5E-2</v>
       </c>
-      <c r="BL239" s="3">
+      <c r="BL239" s="5">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="BM239" s="3">
+      <c r="BM239" s="5">
         <v>0.73799999999999999</v>
       </c>
-      <c r="BN239" s="3">
+      <c r="BN239" s="5">
         <v>0.13300000000000001</v>
       </c>
-      <c r="BO239">
+      <c r="BO239" s="4">
         <v>1.36</v>
       </c>
-      <c r="BP239">
+      <c r="BP239" s="4">
         <v>7.52</v>
       </c>
-      <c r="BQ239" t="s">
+      <c r="BQ239" s="4" t="s">
         <v>1101</v>
       </c>
-      <c r="BR239" t="s">
+      <c r="BR239" s="4" t="s">
         <v>862</v>
       </c>
-      <c r="BS239">
+      <c r="BS239" s="4">
         <v>1.18</v>
       </c>
-      <c r="BT239">
+      <c r="BT239" s="4">
         <v>12.45</v>
       </c>
-      <c r="BU239" t="s">
+      <c r="BU239" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="BV239" t="s">
+      <c r="BV239" s="4" t="s">
         <v>870</v>
       </c>
-      <c r="BW239">
+      <c r="BW239" s="4">
         <v>1.26</v>
       </c>
-      <c r="BX239">
+      <c r="BX239" s="4">
         <v>38.909999999999997</v>
       </c>
-      <c r="BY239" t="s">
+      <c r="BY239" s="4" t="s">
         <v>1227</v>
       </c>
-      <c r="BZ239" t="s">
+      <c r="BZ239" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="CA239">
+      <c r="CA239" s="4">
         <v>1.1599999999999999</v>
       </c>
-      <c r="CB239">
+      <c r="CB239" s="4">
         <v>5.26</v>
       </c>
-      <c r="CC239" t="s">
+      <c r="CC239" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="CD239" t="s">
+      <c r="CD239" s="4" t="s">
         <v>870</v>
       </c>
-      <c r="CE239">
+      <c r="CE239" s="4">
         <v>1.26</v>
       </c>
-      <c r="CF239">
+      <c r="CF239" s="4">
         <v>38.909999999999997</v>
       </c>
-      <c r="CG239" t="s">
+      <c r="CG239" s="4" t="s">
         <v>1227</v>
       </c>
-      <c r="CH239" t="s">
+      <c r="CH239" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="CI239">
+      <c r="CI239" s="4">
         <v>1.1599999999999999</v>
       </c>
-      <c r="CJ239">
+      <c r="CJ239" s="4">
         <v>5.26</v>
       </c>
-      <c r="CK239" t="s">
+      <c r="CK239" s="4" t="s">
         <v>1266</v>
       </c>
     </row>
@@ -77144,7 +77044,10 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" activeCellId="1" sqref="A10:XFD10 A5:XFD5"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -77246,26 +77149,26 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
@@ -77361,72 +77264,72 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>